<commit_message>
major update, if a trip is longer than 90mins then devide it into two different groups
</commit_message>
<xml_diff>
--- a/reservas-adt-3.xlsx
+++ b/reservas-adt-3.xlsx
@@ -501,7 +501,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -544,12 +544,12 @@
         <v>35.7</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -592,12 +592,12 @@
         <v>35.7</v>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -640,12 +640,12 @@
         <v>32.6</v>
       </c>
       <c r="L4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -688,12 +688,12 @@
         <v>32.6</v>
       </c>
       <c r="L5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -736,12 +736,12 @@
         <v>32.6</v>
       </c>
       <c r="L6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -784,12 +784,12 @@
         <v>32.6</v>
       </c>
       <c r="L7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -832,12 +832,12 @@
         <v>32.6</v>
       </c>
       <c r="L8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -880,12 +880,12 @@
         <v>32.6</v>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -928,12 +928,12 @@
         <v>35.7</v>
       </c>
       <c r="L10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -976,12 +976,12 @@
         <v>35.7</v>
       </c>
       <c r="L11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1024,12 +1024,12 @@
         <v>14.9</v>
       </c>
       <c r="L12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1072,12 +1072,12 @@
         <v>14.9</v>
       </c>
       <c r="L13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1120,12 +1120,12 @@
         <v>33.1</v>
       </c>
       <c r="L14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1168,12 +1168,12 @@
         <v>33.1</v>
       </c>
       <c r="L15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1216,12 +1216,12 @@
         <v>34.3</v>
       </c>
       <c r="L16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1264,12 +1264,12 @@
         <v>34.3</v>
       </c>
       <c r="L17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1312,12 +1312,12 @@
         <v>38.9</v>
       </c>
       <c r="L18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1360,12 +1360,12 @@
         <v>38.9</v>
       </c>
       <c r="L19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1408,12 +1408,12 @@
         <v>38.9</v>
       </c>
       <c r="L20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1456,12 +1456,12 @@
         <v>39.8</v>
       </c>
       <c r="L21" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1504,7 +1504,7 @@
         <v>39.8</v>
       </c>
       <c r="L22" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
@@ -1543,13 +1543,13 @@
         <v>963402416</v>
       </c>
       <c r="I23" t="n">
-        <v>19.9</v>
+        <v>19.2</v>
       </c>
       <c r="J23" t="n">
         <v>1</v>
       </c>
       <c r="K23" t="n">
-        <v>19.9</v>
+        <v>19.2</v>
       </c>
       <c r="L23" t="n">
         <v>10</v>
@@ -1927,13 +1927,13 @@
         <v>963402416</v>
       </c>
       <c r="I31" t="n">
-        <v>19.9</v>
+        <v>19.2</v>
       </c>
       <c r="J31" t="n">
         <v>1</v>
       </c>
       <c r="K31" t="n">
-        <v>19.9</v>
+        <v>19.2</v>
       </c>
       <c r="L31" t="n">
         <v>14</v>
@@ -2215,13 +2215,13 @@
         <v>964640040</v>
       </c>
       <c r="I37" t="n">
-        <v>19.8</v>
+        <v>19.9</v>
       </c>
       <c r="J37" t="n">
         <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>19.8</v>
+        <v>19.9</v>
       </c>
       <c r="L37" t="n">
         <v>18</v>

</xml_diff>

<commit_message>
there's two functions left to create, distance matrix and directions
</commit_message>
<xml_diff>
--- a/reservas-adt-3.xlsx
+++ b/reservas-adt-3.xlsx
@@ -1837,7 +1837,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>45.3</v>
+        <v>49.1</v>
       </c>
       <c r="L29" t="n">
         <v>13</v>
@@ -1879,13 +1879,13 @@
         <v>985085668</v>
       </c>
       <c r="I30" t="n">
-        <v>27.8</v>
+        <v>31.6</v>
       </c>
       <c r="J30" t="n">
         <v>2</v>
       </c>
       <c r="K30" t="n">
-        <v>45.3</v>
+        <v>49.1</v>
       </c>
       <c r="L30" t="n">
         <v>13</v>

</xml_diff>